<commit_message>
import dan export tanah gedung fix
</commit_message>
<xml_diff>
--- a/public/templates/template_aset_tanah.xlsx
+++ b/public/templates/template_aset_tanah.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bismillah_sip_aset\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B666ED24-2ACA-4A7D-89AE-E550E0C133E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94680625-F77B-4920-8107-C1BFD84DD5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{D3132774-63BF-4FC5-AB2E-A8A60F82D1E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D3132774-63BF-4FC5-AB2E-A8A60F82D1E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>id_status_aset</t>
   </si>
@@ -460,7 +460,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,8 +548,8 @@
       <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
-        <v>19</v>
+      <c r="K2">
+        <v>0</v>
       </c>
       <c r="L2" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
fix validation sweet alert (kurang handle validasi import excel jika format tidak sesuai)
</commit_message>
<xml_diff>
--- a/public/templates/template_aset_tanah.xlsx
+++ b/public/templates/template_aset_tanah.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bismillah_sip_aset\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F28E2C5-F225-4849-B741-9340F85BD7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C63A611-D519-41DC-A14F-32D829096CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{D3132774-63BF-4FC5-AB2E-A8A60F82D1E5}"/>
   </bookViews>
@@ -459,7 +459,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DFADAA5-72E5-479D-8E65-2F41EB8B7348}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -473,7 +475,7 @@
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -547,7 +549,7 @@
         <v>19</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>200000</v>
       </c>
       <c r="L2" t="s">
         <v>20</v>

</xml_diff>